<commit_message>
fix errors in test_plan
</commit_message>
<xml_diff>
--- a/tests/test_plan_triangle.xlsx
+++ b/tests/test_plan_triangle.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rrcca-my.sharepoint.com/personal/nsidhu10_rrc_ca/Documents/Desktop/rrc_polytech/Intermediate Software Developement/Activities/Activity_02/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="41" documentId="13_ncr:1_{B82F31A6-8AFA-4B46-AE54-0E71FA70719A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EB030A61-1141-4F77-AEED-C2800870F65A}"/>
+  <xr:revisionPtr revIDLastSave="42" documentId="13_ncr:1_{B82F31A6-8AFA-4B46-AE54-0E71FA70719A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{03CF4922-9816-43DD-BC5A-54156CA94F26}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{8D9DD509-55B1-455D-8036-16809AD15960}"/>
   </bookViews>
@@ -272,9 +272,6 @@
     <t>ValueError</t>
   </si>
   <si>
-    <t>The shape color is Green</t>
-  </si>
-  <si>
     <t>Triangle inequality theorm</t>
   </si>
   <si>
@@ -282,6 +279,9 @@
   </si>
   <si>
     <t>Triangle("Green",1,1,11)</t>
+  </si>
+  <si>
+    <t>The shape color is Green,This triangle has three side with length of 9, 10 and 11 centimeters,</t>
   </si>
 </sst>
 </file>
@@ -1146,8 +1146,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DADEBCC4-BB44-48CD-B9AB-1E2FD3EE0EEB}">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A9" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1335,7 +1335,7 @@
         <v>23</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="63.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -1383,13 +1383,13 @@
         <v>9</v>
       </c>
       <c r="C15" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="E15" s="3" t="s">
         <v>31</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>32</v>
       </c>
       <c r="F15" s="3" t="s">
         <v>23</v>

</xml_diff>